<commit_message>
feat: add template transformation
</commit_message>
<xml_diff>
--- a/docs/template_transformation.xlsx
+++ b/docs/template_transformation.xlsx
@@ -91,7 +91,7 @@
     <t>Copiar direto</t>
   </si>
   <si>
-    <t>PARSE_TIMESTAMP(...)</t>
+    <t>to_timestamp(order_datetime, 'YYYY-MM-DD HH24:MI:SS')</t>
   </si>
   <si>
     <t>amount * fx.rate_to_brl</t>
@@ -103,10 +103,10 @@
     <t>JOIN raw_geo_zipcode</t>
   </si>
   <si>
-    <t>JOIN raw_products.sku</t>
-  </si>
-  <si>
-    <t>Relacionar a order_id</t>
+    <t>JOIN stg_products.sku</t>
+  </si>
+  <si>
+    <t>Relacionar com stg_orders.order_id</t>
   </si>
   <si>
     <t>DATE(order_ts)</t>
@@ -151,7 +151,7 @@
     <t>Normalização de data</t>
   </si>
   <si>
-    <t>Conversão de moeda</t>
+    <t>Conversão de moeda para BRL</t>
   </si>
   <si>
     <t>Padronização de e-mail</t>
@@ -160,10 +160,10 @@
     <t>Enriquecimento com geolocalização</t>
   </si>
   <si>
-    <t>Mapeamento produto</t>
-  </si>
-  <si>
-    <t>Mapping entre canais</t>
+    <t>Mapeamento de produto por SKU</t>
+  </si>
+  <si>
+    <t>Resolução de referência polimórfica de pedidos</t>
   </si>
   <si>
     <t>Derivação para métricas diárias</t>

</xml_diff>